<commit_message>
file chooser implemented for the excel
</commit_message>
<xml_diff>
--- a/Dictionary/data.xlsx
+++ b/Dictionary/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>word</t>
   </si>
@@ -29,10 +29,16 @@
     <t>more</t>
   </si>
   <si>
-    <t>good </t>
+    <t>good</t>
   </si>
   <si>
     <t>stuff</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -42,7 +48,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -63,6 +69,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,8 +120,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -129,10 +146,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -155,11 +172,19 @@
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>